<commit_message>
Update Thiết kế giao diện
</commit_message>
<xml_diff>
--- a/Thiết kế/Thiết kế giao diện/Giao Diện.xlsx
+++ b/Thiết kế/Thiết kế giao diện/Giao Diện.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Thiết kế\Thiết kế giao diện\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1B52EB-3D8F-4F66-9686-0AEDD482547A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2259F70-A549-4138-B449-7C1CB0224C21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93EB45F7-56C3-4B7A-8563-2AB1B894BB22}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t>Cb_NhanVien</t>
   </si>
   <si>
-    <t>Combobox</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>Chuyển trang</t>
+  </si>
+  <si>
+    <t>Check Box</t>
   </si>
 </sst>
 </file>
@@ -264,12 +264,12 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,379 +653,379 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9BE349-BC58-4389-A7FE-3D2DE67A1BE9}">
   <dimension ref="A25:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="29.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="29.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>0</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>1</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>2</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>3</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>4</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>5</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>6</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>7</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>8</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>6</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>1</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>2</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>3</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>4</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>5</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>6</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="2" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>9</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>7</v>
-      </c>
-      <c r="B45" s="2" t="s">
+      <c r="D47" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>11</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>12</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>13</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>14</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>8</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>9</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="2" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>15</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>10</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>11</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>12</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>13</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>14</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>15</v>
-      </c>
-      <c r="B53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>